<commit_message>
[Prakash] first cut of DRL Bellman equation assignment
</commit_message>
<xml_diff>
--- a/Sem_2/DRL/asmt1/asmt_1.xlsx
+++ b/Sem_2/DRL/asmt1/asmt_1.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prakash.prasad/Desktop/Sprints/20240122/RL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praka\Acads\M_Tech\new_git_test\BITS-AIML-Mtech-V2\Sem_2\DRL\asmt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AD36C8-FEC7-4A44-93CD-4267F81A53B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79E3B29-2489-4BCC-901B-A009719CA0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="600" windowWidth="28040" windowHeight="17440" xr2:uid="{54824AC5-AB2B-B646-B5C8-C0FC27DC450C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" xr2:uid="{54824AC5-AB2B-B646-B5C8-C0FC27DC450C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="25">
   <si>
     <t>Route</t>
   </si>
@@ -107,12 +107,24 @@
   <si>
     <t>Route_Number</t>
   </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Likelihood*Prior</t>
+  </si>
+  <si>
+    <t>Predictor Prior</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000000000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,16 +139,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -144,21 +170,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,20 +306,81 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="24">
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment vertical="bottom"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -194,16 +395,7 @@
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -212,70 +404,71 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -304,177 +497,6 @@
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0%"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -493,13 +515,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:colOff>30840</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>576942</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
@@ -516,8 +538,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5092700" y="203200"/>
-          <a:ext cx="1803400" cy="1066800"/>
+          <a:off x="4983840" y="201386"/>
+          <a:ext cx="2472873" cy="1057728"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -553,8 +575,137 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1400"/>
-            <a:t>P(c|R) = P(R|c) * P(c)</a:t>
+            <a:t>Posterior</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t> = Likelihood* Prior/ Predictor Prior</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>P(c|R) = P(R|c) * P(c) /</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400"/>
+            <a:t>P(R)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>32655</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>179613</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>201384</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>201385</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AF03C01-EB38-B110-6FCD-F932A8BB5D28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16334012" y="3815442"/>
+          <a:ext cx="2650672" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400"/>
+            <a:t>Inserted</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" baseline="0"/>
+            <a:t> data for laplace smoothing</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" u="sng" baseline="0"/>
+            <a:t>Likelihood:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" baseline="0"/>
+            <a:t>P(R|c) = Count(R,c)+1/</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" baseline="0"/>
+            <a:t>                Count(c)+V</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1400" baseline="0"/>
+            <a:t>V here is num routes : 8</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -563,18 +714,23 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45325.811604282404" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="18" xr:uid="{71DBC164-B416-7842-A43A-FD5638803A31}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Prakash Prasad" refreshedDate="45333.49634247685" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="18" xr:uid="{B362463F-374D-448E-BBB7-AF3897C99457}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E19" sheet="Sheet1"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Route" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8" count="8">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Time" numFmtId="0">
       <sharedItems/>
@@ -601,7 +757,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45325.81331759259" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="21" xr:uid="{A2FDACD9-6F42-FB47-858F-6F3EF72EB9A6}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Prakash Prasad" refreshedDate="45333.496342939812" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="35" xr:uid="{A2FDACD9-6F42-FB47-858F-6F3EF72EB9A6}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="Sheet1"/>
   </cacheSource>
@@ -647,137 +803,6 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="18">
   <r>
-    <n v="1"/>
-    <s v="Best"/>
-    <s v="Minimum"/>
-    <s v="Medium"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="Average"/>
-    <s v="Minimum"/>
-    <s v="Medium"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <s v="Best"/>
-    <s v="Maximum"/>
-    <s v="Low"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="6"/>
-    <s v="Worst"/>
-    <s v="Maximum"/>
-    <s v="High"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="4"/>
-    <s v="Average"/>
-    <s v="Minimum"/>
-    <s v="High"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="Average"/>
-    <s v="Minimum"/>
-    <s v="Low"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <s v="Average"/>
-    <s v="Maximum"/>
-    <s v="High"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="7"/>
-    <s v="Worst"/>
-    <s v="Minimum"/>
-    <s v="High"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <s v="Best"/>
-    <s v="Minimum"/>
-    <s v="Medium"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="Best"/>
-    <s v="Maximum"/>
-    <s v="Medium"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <s v="Worst"/>
-    <s v="Maximum"/>
-    <s v="Medium"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <s v="Best"/>
-    <s v="Minimum"/>
-    <s v="Low"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <s v="Worst"/>
-    <s v="Maximum"/>
-    <s v="High"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="4"/>
-    <s v="Worst"/>
-    <s v="Minimum"/>
-    <s v="Medium"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <s v="Best"/>
-    <s v="Maximum"/>
-    <s v="Low"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="7"/>
-    <s v="Average"/>
-    <s v="Minimum"/>
-    <s v="Low"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="6"/>
-    <s v="Average"/>
-    <s v="Minimum"/>
-    <s v="Low"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="Average"/>
-    <s v="Maximum"/>
-    <s v="Low"/>
-    <x v="1"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="21">
-  <r>
     <x v="0"/>
     <s v="Best"/>
     <s v="Minimum"/>
@@ -903,6 +928,235 @@
     <s v="Low"/>
     <x v="0"/>
   </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="35">
+  <r>
+    <x v="0"/>
+    <s v="Best"/>
+    <s v="Minimum"/>
+    <s v="Medium"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Average"/>
+    <s v="Minimum"/>
+    <s v="Low"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="Average"/>
+    <s v="Maximum"/>
+    <s v="Low"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Average"/>
+    <s v="Minimum"/>
+    <s v="Medium"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="Best"/>
+    <s v="Maximum"/>
+    <s v="Medium"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Best"/>
+    <s v="Maximum"/>
+    <s v="Low"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Worst"/>
+    <s v="Maximum"/>
+    <s v="Medium"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="Best"/>
+    <s v="Maximum"/>
+    <s v="Low"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Average"/>
+    <s v="Minimum"/>
+    <s v="High"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <s v="Worst"/>
+    <s v="Minimum"/>
+    <s v="Medium"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Average"/>
+    <s v="Maximum"/>
+    <s v="High"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <s v="Worst"/>
+    <s v="Maximum"/>
+    <s v="High"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Worst"/>
+    <s v="Maximum"/>
+    <s v="High"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <s v="Average"/>
+    <s v="Minimum"/>
+    <s v="Low"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Worst"/>
+    <s v="Minimum"/>
+    <s v="High"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <s v="Average"/>
+    <s v="Minimum"/>
+    <s v="Low"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="Best"/>
+    <s v="Minimum"/>
+    <s v="Medium"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <s v="Best"/>
+    <s v="Minimum"/>
+    <s v="Low"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+  </r>
   <r>
     <x v="8"/>
     <m/>
@@ -928,8 +1182,187 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A065725-16D5-284B-A54D-F709731E8293}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Route_Number">
-  <location ref="I2:L17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B328DB16-4992-4C53-87BC-5C1F2A304E77}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Class">
+  <location ref="F8:G11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Prior" fld="0" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="8">
+    <format dxfId="7">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="4" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{67C1F4F5-BA47-462C-8996-03BCBF3B23E6}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Route">
+  <location ref="F14:G23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Predictor Prior" fld="1" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5A663BB-1ACA-4098-8B70-C6E7059B019A}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Route_Number">
+  <location ref="I2:K17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
       <items count="10">
@@ -947,7 +1380,7 @@
     </pivotField>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
         <item x="1"/>
@@ -1011,18 +1444,15 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="3">
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
   </colItems>
-  <dataFields count="3">
+  <dataFields count="2">
     <dataField name="Counts" fld="1" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Likelihood" fld="2" subtotal="count" baseField="0" baseItem="0" numFmtId="10">
       <extLst>
@@ -1031,10 +1461,9 @@
         </ext>
       </extLst>
     </dataField>
-    <dataField name="Posterior" fld="3" subtotal="count" showDataAs="percentOfCol" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
-  <formats count="17">
-    <format dxfId="94">
+  <formats count="13">
+    <format dxfId="23">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1046,7 +1475,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="22">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1065,7 +1494,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="21">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1077,7 +1506,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="20">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="3">
           <reference field="4294967294" count="1" selected="0">
@@ -1098,7 +1527,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="19">
       <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1107,33 +1536,45 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="74">
-      <pivotArea outline="0" fieldPosition="0">
+    <format dxfId="18">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="2"/>
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
+    <format dxfId="17">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
           <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="1">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
+        <references count="2">
           <reference field="0" count="5">
             <x v="0"/>
             <x v="2"/>
@@ -1147,24 +1588,25 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+    <format dxfId="13">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
-          <reference field="4294967294" count="1" selected="0">
+          <reference field="0" count="5">
+            <x v="0"/>
             <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="7"/>
           </reference>
-          <reference field="4" count="1">
-            <x v="1"/>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
+        <references count="2">
           <reference field="0" count="7">
             <x v="0"/>
             <x v="1"/>
@@ -1180,121 +1622,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
-      <pivotArea field="4" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="7">
+            <x v="0"/>
+            <x v="1"/>
             <x v="2"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
           </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="52">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="51">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="37">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
+          <reference field="4" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
       </pivotArea>
-    </format>
-    <format dxfId="36">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="20">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF8B324A-C60F-224F-8D7C-2B4BBE6BF308}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Class">
-  <location ref="F11:G14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Prior" fld="1" subtotal="count" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="9"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="98">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -1606,75 +1950,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F774B3C-6915-B544-B66A-27C11DDFFB61}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.0703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.35546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.35546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="4"/>
+    <col min="19" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="S2" s="18">
+        <v>1</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="28">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1686,24 +2052,36 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="5">
         <v>7</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>0.3888888888888889</v>
       </c>
-      <c r="L3" s="7">
-        <v>0.3888888888888889</v>
+      <c r="S3" s="21">
+        <v>2</v>
+      </c>
+      <c r="T3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="23" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A4" s="28">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -1715,25 +2093,44 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="30">
         <v>1</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="31">
         <v>1</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="32">
         <v>0.14285714285714285</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="32">
+        <f>K4*$G$9</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="M4" s="5"/>
+      <c r="M4" s="33">
+        <f>L4/VLOOKUP(I4,$F$15:$G$22,2,0)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="S4" s="21">
+        <v>3</v>
+      </c>
+      <c r="T4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="23" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A5" s="28">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1745,24 +2142,44 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="34">
         <v>3</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="5">
         <v>2</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>0.2857142857142857</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
+        <f>K5*$G$9</f>
         <v>0.1111111111111111</v>
       </c>
+      <c r="M5" s="35">
+        <f t="shared" ref="M5:M8" si="0">L5/VLOOKUP(I5,$F$15:$G$22,2,0)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="S5" s="21">
+        <v>4</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W5" s="23" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A6" s="28">
         <v>2</v>
       </c>
       <c r="B6" t="s">
@@ -1774,24 +2191,44 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="34">
         <v>4</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="5">
         <v>2</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>0.2857142857142857</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="6">
+        <f>K6*$G$9</f>
         <v>0.1111111111111111</v>
       </c>
+      <c r="M6" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S6" s="21">
+        <v>5</v>
+      </c>
+      <c r="T6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A7" s="28">
         <v>3</v>
       </c>
       <c r="B7" t="s">
@@ -1803,24 +2240,44 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="34">
         <v>5</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="5">
         <v>1</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>0.14285714285714285</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
+        <f>K7*$G$9</f>
         <v>5.5555555555555552E-2</v>
       </c>
+      <c r="M7" s="35">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="21">
+        <v>6</v>
+      </c>
+      <c r="T7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W7" s="23" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="28">
         <v>3</v>
       </c>
       <c r="B8" t="s">
@@ -1832,24 +2289,50 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="4">
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="36">
         <v>8</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="37">
         <v>1</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="38">
         <v>0.14285714285714285</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="38">
+        <f>K8*$G$9</f>
         <v>5.5555555555555552E-2</v>
       </c>
+      <c r="M8" s="39">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="S8" s="21">
+        <v>7</v>
+      </c>
+      <c r="T8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W8" s="23" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="28">
         <v>3</v>
       </c>
       <c r="B9" t="s">
@@ -1861,24 +2344,44 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="12" t="s">
         <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.3888888888888889</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="5">
         <v>11</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>0.61111111111111116</v>
       </c>
-      <c r="L9" s="7">
-        <v>0.61111111111111116</v>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="S9" s="21">
+        <v>8</v>
+      </c>
+      <c r="T9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W9" s="23" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A10" s="28">
         <v>4</v>
       </c>
       <c r="B10" t="s">
@@ -1890,24 +2393,50 @@
       <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="4">
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="I10" s="30">
         <v>1</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="31">
         <v>2</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="32">
         <v>0.18181818181818182</v>
       </c>
-      <c r="L10" s="7">
-        <v>0.1111111111111111</v>
+      <c r="L10" s="32">
+        <f>K10*$G$10</f>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="M10" s="33">
+        <f>L10/VLOOKUP(I10,$F$15:$G$22,2,0)</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="S10" s="21">
+        <v>1</v>
+      </c>
+      <c r="T10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W10" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A11" s="28">
         <v>4</v>
       </c>
       <c r="B11" t="s">
@@ -1919,30 +2448,50 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="4">
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="34">
         <v>2</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="5">
         <v>2</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>0.18181818181818182</v>
       </c>
-      <c r="L11" s="7">
-        <v>0.1111111111111111</v>
+      <c r="L11" s="6">
+        <f t="shared" ref="L11:L16" si="1">K11*$G$10</f>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="M11" s="35">
+        <f t="shared" ref="M11:M16" si="2">L11/VLOOKUP(I11,$F$15:$G$22,2,0)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="S11" s="21">
+        <v>2</v>
+      </c>
+      <c r="T11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W11" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A12" s="28">
         <v>5</v>
       </c>
       <c r="B12" t="s">
@@ -1954,30 +2503,44 @@
       <c r="D12" t="s">
         <v>13</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="I12" s="34">
+        <v>3</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="M12" s="35">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="S12" s="21">
+        <v>3</v>
+      </c>
+      <c r="T12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="3">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="I12" s="4">
-        <v>3</v>
-      </c>
-      <c r="J12" s="8">
-        <v>1</v>
-      </c>
-      <c r="K12" s="7">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="L12" s="7">
-        <v>5.5555555555555552E-2</v>
-      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A13" s="28">
         <v>5</v>
       </c>
       <c r="B13" t="s">
@@ -1989,30 +2552,44 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.61111111111111116</v>
-      </c>
-      <c r="I13" s="4">
+      <c r="I13" s="34">
         <v>5</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="5">
         <v>1</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="L13" s="7">
-        <v>5.5555555555555552E-2</v>
+      <c r="L13" s="6">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="M13" s="35">
+        <f t="shared" si="2"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="S13" s="21">
+        <v>4</v>
+      </c>
+      <c r="T13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W13" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A14" s="28">
         <v>6</v>
       </c>
       <c r="B14" t="s">
@@ -2024,30 +2601,50 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-      <c r="I14" s="4">
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="34">
         <v>6</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="5">
         <v>2</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>0.18181818181818182</v>
       </c>
-      <c r="L14" s="7">
-        <v>0.1111111111111111</v>
+      <c r="L14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="M14" s="35">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="S14" s="21">
+        <v>5</v>
+      </c>
+      <c r="T14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W14" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A15" s="28">
         <v>6</v>
       </c>
       <c r="B15" t="s">
@@ -2059,24 +2656,50 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="4">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I15" s="34">
         <v>7</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="5">
         <v>2</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>0.18181818181818182</v>
       </c>
-      <c r="L15" s="7">
-        <v>0.1111111111111111</v>
+      <c r="L15" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11111111111111112</v>
+      </c>
+      <c r="M15" s="35">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="S15" s="21">
+        <v>6</v>
+      </c>
+      <c r="T15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="28">
         <v>7</v>
       </c>
       <c r="B16" t="s">
@@ -2088,24 +2711,50 @@
       <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="4">
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="I16" s="36">
         <v>8</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="37">
         <v>1</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="38">
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="L16" s="7">
-        <v>5.5555555555555552E-2</v>
+      <c r="L16" s="38">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="M16" s="39">
+        <f t="shared" si="2"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="S16" s="21">
+        <v>7</v>
+      </c>
+      <c r="T16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="W16" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="28">
         <v>7</v>
       </c>
       <c r="B17" t="s">
@@ -2117,24 +2766,42 @@
       <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="12" t="s">
         <v>7</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.16666666666666666</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="5">
         <v>18</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>1</v>
       </c>
-      <c r="L17" s="7">
-        <v>1</v>
+      <c r="S17" s="24">
+        <v>8</v>
+      </c>
+      <c r="T17" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="V17" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="W17" s="26" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A18" s="28">
         <v>8</v>
       </c>
       <c r="B18" t="s">
@@ -2146,25 +2813,74 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="12" t="s">
         <v>11</v>
       </c>
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.1111111111111111</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:23" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="29">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="14" t="s">
         <v>7</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="F20" s="2">
+        <v>6</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="F21" s="2">
+        <v>7</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="F22" s="2">
+        <v>8</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="F23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2172,6 +2888,6 @@
     <sortCondition ref="A2:A20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>